<commit_message>
HRT lit review, rearranged article order
</commit_message>
<xml_diff>
--- a/references/OtherStudies20150501.xlsx
+++ b/references/OtherStudies20150501.xlsx
@@ -63,9 +63,6 @@
     <t>97,638 women in NIH-AARP cohort, both questionnaires</t>
   </si>
   <si>
-    <t>Strengths/Limitations</t>
-  </si>
-  <si>
     <t>MHT</t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>no childhood residential information, number of sunburns, no skin sunburn reactions, or number of nevi</t>
+  </si>
+  <si>
+    <t>Limitations</t>
   </si>
 </sst>
 </file>
@@ -664,11 +664,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -690,303 +690,306 @@
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7"/>
       <c r="D2" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="150" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>3</v>
+        <v>75</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>5</v>
+        <v>39</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9"/>
     </row>
-    <row r="5" spans="1:12" ht="150" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9"/>
     </row>
-    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>26</v>
+        <v>67</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
     </row>
-    <row r="9" spans="1:12" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>66</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9"/>
     </row>
     <row r="11" spans="1:12" ht="75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="9"/>
     </row>
-    <row r="13" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="4" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="7"/>
-      <c r="D14" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="112.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="3" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" spans="1:12" s="4" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="7"/>
+      <c r="D15" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="112.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="9"/>
-    </row>
-    <row r="17" spans="1:10" ht="150" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    </row>
+    <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="9"/>
+    </row>
+    <row r="18" spans="1:10" ht="150" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="1:10" ht="112.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="9"/>
+    </row>
+    <row r="22" spans="1:10" ht="75" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="9"/>
-    </row>
-    <row r="19" spans="1:10" ht="112.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="9"/>
-    </row>
-    <row r="21" spans="1:10" ht="75" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="9"/>
-    </row>
-    <row r="23" spans="1:10" ht="112.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+    </row>
+    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="9"/>
+    </row>
+    <row r="24" spans="1:10" ht="112.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
create base/risk merge/var SAS files, updated all 4 with header, and title edits
</commit_message>
<xml_diff>
--- a/references/OtherStudies20150501.xlsx
+++ b/references/OtherStudies20150501.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>Outcome</t>
   </si>
@@ -141,9 +141,6 @@
     <t xml:space="preserve">cox proportional hazards with age as time-scale, birth baseline 5 yrs, gender, alcohol intake, years smoked, skin pigmentation, hair colo, personal history of non melanom skin cancer, decades worked, education, proxy childhood and adjust UVR                                </t>
   </si>
   <si>
-    <t>Melanoma risk not associated with age at menarche, age at first use of oral contraceptives, age at first birth, parity, meno status, or HRT use, height, weight, BMI or mean;</t>
-  </si>
-  <si>
     <t>Liu T, 1996, Surg Clin NA</t>
   </si>
   <si>
@@ -256,6 +253,18 @@
   </si>
   <si>
     <t>Limitations</t>
+  </si>
+  <si>
+    <t>Melanoma risk not associated with age at menarche, age at first use of oral contraceptives, age at first birth, parity, meno status, or HRT use, height, weight, BMI</t>
+  </si>
+  <si>
+    <t>parity, age at first birth</t>
+  </si>
+  <si>
+    <t>oral contraceptive use and duration</t>
+  </si>
+  <si>
+    <t>IJE</t>
   </si>
 </sst>
 </file>
@@ -690,54 +699,54 @@
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7"/>
       <c r="D2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="150" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>36</v>
@@ -746,28 +755,28 @@
         <v>37</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>38</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -777,6 +786,9 @@
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="B5" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
@@ -784,10 +796,13 @@
         <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>9</v>
+        <v>80</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>24</v>
@@ -801,10 +816,10 @@
     </row>
     <row r="7" spans="1:12" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -812,19 +827,19 @@
     </row>
     <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -832,10 +847,10 @@
     </row>
     <row r="11" spans="1:12" ht="75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>33</v>
@@ -852,10 +867,10 @@
     </row>
     <row r="13" spans="1:12" ht="75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>1</v>
@@ -876,7 +891,7 @@
     <row r="15" spans="1:12" s="4" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7"/>
       <c r="D15" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="112.5" x14ac:dyDescent="0.3">
@@ -967,25 +982,25 @@
     </row>
     <row r="24" spans="1:10" ht="112.5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>